<commit_message>
combined login and invalid login tests into login class
</commit_message>
<xml_diff>
--- a/cybertron/input/xlData.xlsx
+++ b/cybertron/input/xlData.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17835" windowHeight="10710" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21315" windowHeight="5940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
-    <sheet name="error" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
+  <oleSize ref="A1:Q17"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>username</t>
   </si>
@@ -29,6 +29,24 @@
   </si>
   <si>
     <t>facebook@123</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>Expected</t>
+  </si>
+  <si>
+    <t>The password that you've entered is incorrect</t>
+  </si>
+  <si>
+    <t>POSITIVE</t>
+  </si>
+  <si>
+    <t>NEGATIVE</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -88,10 +106,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -401,80 +420,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="A1:B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="42.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>8667058239</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>8667058239</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1234</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BE1B087-27EA-4938-A18B-3D1ECEAD751C}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>8667058239</v>
-      </c>
-      <c r="B2" s="2">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="facebook@123" xr:uid="{728C529B-AB01-4149-86B5-221A2D45B61F}"/>
+    <hyperlink ref="B3" r:id="rId2" display="facebook@123" xr:uid="{5994AD0A-8BCE-424D-92D9-05586318CF6A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
wrong email test case included
</commit_message>
<xml_diff>
--- a/cybertron/input/xlData.xlsx
+++ b/cybertron/input/xlData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21315" windowHeight="5940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21315" windowHeight="2640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>username</t>
   </si>
@@ -47,6 +47,12 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>sdf</t>
+  </si>
+  <si>
+    <t>The email address or phone number that you've entered doesn't match any account</t>
   </si>
 </sst>
 </file>
@@ -420,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,10 +483,25 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B3" r:id="rId2" display="facebook@123" xr:uid="{5994AD0A-8BCE-424D-92D9-05586318CF6A}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{ACFC56DB-F3B4-4E4D-9A02-8D39943EBABB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Assert Statement for Valid Login
</commit_message>
<xml_diff>
--- a/cybertron/input/xlData.xlsx
+++ b/cybertron/input/xlData.xlsx
@@ -10,7 +10,6 @@
     <sheet name="login" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
-  <oleSize ref="A1:Q17"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -46,13 +45,13 @@
     <t>NEGATIVE</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>sdf</t>
   </si>
   <si>
     <t>The email address or phone number that you've entered doesn't match any account</t>
+  </si>
+  <si>
+    <t>Facebook</t>
   </si>
 </sst>
 </file>
@@ -112,11 +111,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -429,7 +427,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,10 +446,10 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -462,11 +460,11 @@
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>8</v>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -476,7 +474,7 @@
       <c r="B3" s="2">
         <v>1234</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -484,17 +482,17 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>9</v>
+      <c r="A4" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>10</v>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>